<commit_message>
add ExecResult.Insights  if cond Match count and analyzed datarow count
</commit_message>
<xml_diff>
--- a/2-Tests/Lexerow.Core.Tests/10-Files/ForIfThenSetNullBasic.xlsx
+++ b/2-Tests/Lexerow.Core.Tests/10-Files/ForIfThenSetNullBasic.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a990f455bb745add/ProjetsDev/10-Pierlam/Lexerow/Dev/LexerowSol/2-Tests/Lexerow.Core.Tests/10-Files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a990f455bb745add/ProjetsDev/10-Pierlam/Lexerow/Dev/Lexerow/2-Tests/Lexerow.Core.Tests/10-Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="11_AD4DB114E441178AC67DF4536695FF58683EDF1B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D23AD420-4908-4825-946D-B1F9F9F4A8C8}"/>
+  <xr:revisionPtr revIDLastSave="27" documentId="11_AD4DB114E441178AC67DF4536695FF58683EDF1B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AD0DFD62-E981-444E-B4AE-7CD1E9ABAD00}"/>
   <bookViews>
-    <workbookView xWindow="3930" yWindow="2925" windowWidth="24150" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7920" yWindow="2715" windowWidth="17535" windowHeight="11355" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
   <si>
     <t>notmodified</t>
   </si>
@@ -40,6 +40,12 @@
   </si>
   <si>
     <t>toclear</t>
+  </si>
+  <si>
+    <t>Text</t>
+  </si>
+  <si>
+    <t>warning</t>
   </si>
 </sst>
 </file>
@@ -93,10 +99,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -362,10 +364,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -415,6 +417,17 @@
         <v>1</v>
       </c>
     </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>